<commit_message>
[ADD] CheatKey, RangeEnemy, MainScene, Ranking, FireBall
많은 것
</commit_message>
<xml_diff>
--- a/ActionGame/Seuol_CheckList.xlsx
+++ b/ActionGame/Seuol_CheckList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lomil\Desktop\Git\ActionGame\ActionGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lomi1\Desktop\Git\ActionGame\ActionGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>플레이어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -281,10 +281,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6시간</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2시간47분</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -298,6 +294,42 @@
   </si>
   <si>
     <t>17분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7분 6초</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1시간 7분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1시간 7분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메뉴화면 구성 2시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25분 46초</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1010,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1082,7 +1114,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>21</v>
@@ -1111,14 +1143,16 @@
       <c r="K4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="24" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>22</v>
@@ -1145,14 +1179,14 @@
       <c r="K5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>23</v>
@@ -1177,13 +1211,15 @@
       <c r="K6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="7"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="10" t="s">
         <v>42</v>
       </c>
@@ -1195,15 +1231,19 @@
       <c r="G7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="7"/>
+      <c r="J7" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="K7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="7"/>
+      <c r="L7" s="26"/>
     </row>
     <row r="8" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -1213,14 +1253,16 @@
       <c r="C8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>67</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
       <c r="G8" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>13</v>
@@ -1231,9 +1273,7 @@
       <c r="K8" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="L8" s="26"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
@@ -1253,11 +1293,13 @@
       <c r="I9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="K9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="7"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
@@ -1273,11 +1315,13 @@
       <c r="I10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="7"/>
+      <c r="J10" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="K10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="7"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
@@ -1291,11 +1335,13 @@
       <c r="I11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>68</v>
+      </c>
       <c r="K11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="7"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
@@ -1317,10 +1363,16 @@
       </c>
       <c r="L12" s="9"/>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="J4:J6"/>
+    <mergeCell ref="L4:L11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>